<commit_message>
Changed class filenames as per tests
</commit_message>
<xml_diff>
--- a/src/main/DataFromExcel/userData.xlsx
+++ b/src/main/DataFromExcel/userData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuchander\Api_testing_maven\src\main\DataFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB7B97C-1971-4A1F-B7A5-46CEE7E313F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8251B850-0045-4ECF-B6BB-E290FED0C60D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>supriya12345</t>
+  </si>
+  <si>
+    <t>lakshmi</t>
+  </si>
+  <si>
+    <t>lakshmi12@gmail.com</t>
+  </si>
+  <si>
+    <t>lakshmi12345</t>
   </si>
 </sst>
 </file>
@@ -919,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,14 +1011,29 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{18FDF94F-6EF1-4A65-B982-220A26B884D7}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E0DBBD28-56A8-4B7C-803D-FFD25EE2D5F9}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{798ECF53-6585-4A8C-93FD-21D3BB341E8C}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{2E1B9A85-CD6B-4D30-A462-310257480E0E}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{3183B3D7-39AB-4671-84D2-9289617DB527}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>